<commit_message>
adding CDOM data processing R code
</commit_message>
<xml_diff>
--- a/processing_scripts/CDOM/TMP3_and_monthly_processed/TMP3_and_monthly_aqualog_metadata_corrected.xlsx
+++ b/processing_scripts/CDOM/TMP3_and_monthly_processed/TMP3_and_monthly_aqualog_metadata_corrected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimj704/Github/TEMPEST_Porewater/processing_scripts/CDOM/TMP3_monthly_processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimj704/Github/TEMPEST_Porewater/processing_scripts/CDOM/TMP3_and_monthly_processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3DDCA9-497D-1B4A-B407-D3F72F04574D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B98F131-90C0-4F47-97A2-77A8C8561C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-180" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="1500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -1038,9 +1038,6 @@
     <t>pstT04Jun25</t>
   </si>
   <si>
-    <t>mis-named on Aqualog as H43 (02) - should be H6</t>
-  </si>
-  <si>
     <t>SSW611AF2s</t>
   </si>
   <si>
@@ -1078,6 +1075,9 @@
   </si>
   <si>
     <t>DOC is not accurate</t>
+  </si>
+  <si>
+    <t>mis-named on Aqualog as H3 (02) - should be H6</t>
   </si>
 </sst>
 </file>
@@ -1973,7 +1973,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2021,10 +2021,10 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>344</v>
+      </c>
+      <c r="N1" t="s">
         <v>345</v>
-      </c>
-      <c r="N1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2220,7 +2220,7 @@
         <v>114</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2508,7 +2508,7 @@
         <v>122</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3768,7 +3768,7 @@
         <v>155</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E50">
         <v>2</v>
@@ -3790,7 +3790,7 @@
         <v>5.7990000000000004</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M50">
         <v>3</v>
@@ -3865,7 +3865,7 @@
         <v>3.641</v>
       </c>
       <c r="L52" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M52">
         <v>3</v>
@@ -3904,7 +3904,7 @@
         <v>4.3849999999999998</v>
       </c>
       <c r="L53" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M53">
         <v>3</v>
@@ -4159,7 +4159,7 @@
         <v>6.34</v>
       </c>
       <c r="L60" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M60" s="7">
         <v>3</v>
@@ -4212,7 +4212,7 @@
         <v>164</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -4234,7 +4234,7 @@
         <v>6.7</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M62">
         <v>3</v>
@@ -4251,7 +4251,7 @@
         <v>165</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -4273,7 +4273,7 @@
         <v>5.8460000000000001</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M63">
         <v>3</v>
@@ -5329,7 +5329,7 @@
         <v>4.7190000000000003</v>
       </c>
       <c r="L92" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M92">
         <v>3</v>
@@ -5369,7 +5369,7 @@
         <v>6.3150000000000004</v>
       </c>
       <c r="L93" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M93">
         <v>3</v>
@@ -5423,7 +5423,7 @@
         <v>201</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E95">
         <v>2</v>
@@ -5445,7 +5445,7 @@
         <v>9.5549999999999997</v>
       </c>
       <c r="L95" s="7" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="M95">
         <v>3</v>
@@ -6669,7 +6669,7 @@
         <v>6.6680000000000001</v>
       </c>
       <c r="L128" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M128">
         <v>3</v>
@@ -8521,7 +8521,7 @@
         <v>18.61</v>
       </c>
       <c r="L178" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M178">
         <v>0.7</v>
@@ -8820,7 +8820,7 @@
         <v>60.4</v>
       </c>
       <c r="L186" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M186">
         <v>0.2</v>

</xml_diff>